<commit_message>
Valores estimados de cotizacion parcial
</commit_message>
<xml_diff>
--- a/Cotizaciones/Cotizaciones.xlsx
+++ b/Cotizaciones/Cotizaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megam\Videos\Proyectos\Extrusor\Cotizaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84BAEBF2-45D0-489C-9DFA-5813BC20C218}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E154048F-B2A1-4804-967D-AF4CD1D100B4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" xr2:uid="{D60FC618-7C1D-4E12-B1EA-D4CBAE960DFB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" firstSheet="2" activeTab="3" xr2:uid="{D60FC618-7C1D-4E12-B1EA-D4CBAE960DFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Mecánica " sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t xml:space="preserve">DESCRIPCION </t>
   </si>
@@ -45,9 +45,6 @@
     <t>COTIZACION DE MATERIALES</t>
   </si>
   <si>
-    <t xml:space="preserve">Husillo </t>
-  </si>
-  <si>
     <t>Camisa</t>
   </si>
   <si>
@@ -69,16 +66,61 @@
     <t>variador de velocidad</t>
   </si>
   <si>
-    <t xml:space="preserve">motor electrico </t>
-  </si>
-  <si>
-    <t>caja reductora</t>
-  </si>
-  <si>
     <t xml:space="preserve">Total </t>
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Husillo para extrusora de 21 filetes y 45 mm de diametro</t>
+  </si>
+  <si>
+    <t>Motoreductor de 36 rpm</t>
+  </si>
+  <si>
+    <t>https://articulo.mercadolibre.com.co/MCO-464719278-motor-reductor-marca-sew-36-rpm-075-kw-_JM</t>
+  </si>
+  <si>
+    <t>https://www.industrialshields.com/es/product/din-rail-power-supply-ac-dc-30w-2-output-1-3a-at-24vdc/</t>
+  </si>
+  <si>
+    <t>pulsador de inicio</t>
+  </si>
+  <si>
+    <t>Pulsador de paro</t>
+  </si>
+  <si>
+    <t>boton paro de emergencia</t>
+  </si>
+  <si>
+    <t>https://articulo.mercadolibre.com.co/MCO-467371151-boton-interruptor-de-parada-de-emergencia-ac-660v-10a-rojo-_JM</t>
+  </si>
+  <si>
+    <t>https://www.vistronica.com/conectores-cables-y-switches/interruptor-pulsador-normalmente-abierto-rojo-amarillo-detail.html</t>
+  </si>
+  <si>
+    <t>https://www.vistronica.com/conectores-cables-y-switches/interruptor-pulsador-normalmente-abierto-22mm-la38-11bn-verde-detail.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">luz piloto para indicacion de inicio, paro </t>
+  </si>
+  <si>
+    <t>https://articulo.mercadolibre.com.co/MCO-459758466-indicador-de-luz-led-senal-piloto-5pcs-rojo-verde-azul-_JM</t>
+  </si>
+  <si>
+    <t>sensor de temperatura</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/2-Big-Chief-BC21152A-850W-2-Heating-Bands-120-VAC-19123/122485226796?hash=item1c84b03d2c:g:xywAAOSwnHZYb44b</t>
+  </si>
+  <si>
+    <t>https://articulo.mercadolibre.com.co/MCO-467314259-variador-de-velocidad-danfoss-vlt-micro-drive-1hp-220vac-_JM</t>
+  </si>
+  <si>
+    <t>automatico de seguridad</t>
+  </si>
+  <si>
+    <t>https://www.vistronica.com/sensores/temperatura/termocupla-tipo-e-son-sonda-de-rosca-m6-50cm-detail.html</t>
   </si>
 </sst>
 </file>
@@ -121,7 +163,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -130,17 +172,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -345,6 +376,58 @@
       </right>
       <top/>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -353,51 +436,113 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,10 +857,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1920B3B7-81A7-401C-9988-F03B36BDE3F4}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,85 +869,80 @@
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="97" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="38" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="7">
+        <v>500000</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="6"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="12">
-        <f>SUM(B4:B7)</f>
+      <c r="A7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="39">
+        <f>SUM(B3:B6)</f>
+        <v>500000</v>
+      </c>
+      <c r="C7" s="24">
+        <f>SUM(C4:C6)</f>
         <v>0</v>
       </c>
-      <c r="C8" s="12">
-        <f>SUM(C4:C7)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="16">
-        <f>B8+C8</f>
-        <v>0</v>
+      <c r="D7" s="40">
+        <f>B7+C7</f>
+        <v>500000</v>
       </c>
     </row>
   </sheetData>
@@ -809,6 +950,7 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -817,7 +959,8 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,61 +968,74 @@
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="96.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="12">
+        <v>454226.3</v>
+      </c>
+      <c r="C3">
+        <v>117762.37</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="14"/>
+      <c r="B4" s="12">
+        <v>156623</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="12">
+      <c r="A5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="24">
         <f>SUM(B1:B4)</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="12">
+        <v>610849.30000000005</v>
+      </c>
+      <c r="C5" s="24">
         <f>SUM(C1:C4)</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="12">
+        <v>117762.37</v>
+      </c>
+      <c r="D5" s="24">
         <f>B5+C5</f>
-        <v>0</v>
+        <v>728611.67</v>
       </c>
     </row>
   </sheetData>
@@ -896,82 +1052,103 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="96.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="30" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="46">
+        <v>49046</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="B4" s="12">
+        <v>750000</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="7">
+        <v>550000</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="47">
+        <v>11900</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="15"/>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="12">
+      <c r="B7" s="43">
         <f>SUM(B3:B6)</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="12">
+        <v>1360946</v>
+      </c>
+      <c r="C7" s="43">
         <f>SUM(C3:C6)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="44">
         <f>B7+C7</f>
-        <v>0</v>
+        <v>1360946</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -985,12 +1162,126 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C90FDA-D243-4282-B9E7-451526262F2C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="97.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="12">
+        <v>8330</v>
+      </c>
+      <c r="C3" s="41">
+        <v>9200</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="12">
+        <v>8330</v>
+      </c>
+      <c r="C4" s="41">
+        <v>9200</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="12">
+        <v>18000</v>
+      </c>
+      <c r="C5" s="12">
+        <v>9800</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="12">
+        <v>44990</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="12">
+        <v>30000</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="45"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="24">
+        <f>SUM(B1:B4)</f>
+        <v>16660</v>
+      </c>
+      <c r="C8" s="24">
+        <f>SUM(C1:C4)</f>
+        <v>18400</v>
+      </c>
+      <c r="D8" s="24">
+        <f>B8+C8</f>
+        <v>35060</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>